<commit_message>
Updated comment that was wrong
</commit_message>
<xml_diff>
--- a/uft-one-ppm-executive-build-test/Default.xlsx
+++ b/uft-one-ppm-executive-build-test/Default.xlsx
@@ -181,9 +181,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -194,7 +192,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -536,10 +536,10 @@
       </c>
     </row>
     <row>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the step to click the Done button when looking into changing from the calculated risk to the override value
</commit_message>
<xml_diff>
--- a/uft-one-ppm-executive-build-test/Default.xlsx
+++ b/uft-one-ppm-executive-build-test/Default.xlsx
@@ -181,7 +181,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -192,9 +194,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -536,10 +536,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>1</v>
       </c>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated impoper syntax in the Exit Do
</commit_message>
<xml_diff>
--- a/uft-one-ppm-executive-build-test/Default.xlsx
+++ b/uft-one-ppm-executive-build-test/Default.xlsx
@@ -181,9 +181,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -194,7 +192,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -536,10 +536,10 @@
       </c>
     </row>
     <row>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ClickLoop function to leverage it, removed duplicative code Added traditional OR click to force autoscroll if the resolution is too low on the UFT machine to have the 2nd verified dashboard to be displayed, plus changed the selection of the hamburger_menu to be VRI off of the dashboard title.
</commit_message>
<xml_diff>
--- a/uft-one-ppm-executive-build-test/Default.xlsx
+++ b/uft-one-ppm-executive-build-test/Default.xlsx
@@ -181,9 +181,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -194,7 +192,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -536,10 +536,10 @@
       </c>
     </row>
     <row>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated manual reporter event error handling
</commit_message>
<xml_diff>
--- a/uft-one-ppm-executive-build-test/Default.xlsx
+++ b/uft-one-ppm-executive-build-test/Default.xlsx
@@ -181,7 +181,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -192,9 +194,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -536,10 +536,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>1</v>
       </c>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated to handle changes coming in UFT One 15.0.2 Commented out the msgbox, which can cause UFT One to be in a locked state when executed from Jenkins
</commit_message>
<xml_diff>
--- a/uft-one-ppm-executive-build-test/Default.xlsx
+++ b/uft-one-ppm-executive-build-test/Default.xlsx
@@ -181,9 +181,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -194,7 +192,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -536,10 +536,10 @@
       </c>
     </row>
     <row>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated ClickLoop to gracefully abort if failure number reached Updated failure abort to be 3 instead of 90
</commit_message>
<xml_diff>
--- a/uft-one-ppm-executive-build-test/Default.xlsx
+++ b/uft-one-ppm-executive-build-test/Default.xlsx
@@ -181,7 +181,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -192,9 +194,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -536,10 +536,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>1</v>
       </c>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
You can use the public PPM demo http://ppmdemo.mfadvantageinc.com/menu.html and this will work, edit data table if you want to run against nimbusserver Added logic to enumerate handled browsers, script as is will fail on 2nd iteration on purpose Updated to exclusively use AI-based object recognition, script will no longer function in 15.0.1 Working with R&D on autoscroll issue, uncomment the commented code if it fails.
</commit_message>
<xml_diff>
--- a/uft-one-ppm-executive-build-test/Default.xlsx
+++ b/uft-one-ppm-executive-build-test/Default.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>BrowserName</t>
   </si>
@@ -23,10 +23,16 @@
     <t>CHROME</t>
   </si>
   <si>
-    <t>http://nimbusserver.aos.com:8088/menu.html</t>
+    <t>http://nimbusserver.aos.com:8088</t>
+  </si>
+  <si>
+    <t>MSEDGE</t>
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>http://ppmdemo.mfadvantageinc.com/menu.html</t>
   </si>
 </sst>
 </file>
@@ -514,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -523,7 +529,7 @@
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.8359375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -532,12 +538,20 @@
         <v>0</v>
       </c>
       <c t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row>
       <c s="3" t="s">
         <v>1</v>
+      </c>
+      <c s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row>
+      <c s="3" t="s">
+        <v>3</v>
       </c>
       <c s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
R&D determined that the root cause of the autoscroll issue is PPM has a W3C violation, they will research how to have UFT AI autoscroll work in this circumstance Updated to point back to the Nimbus instance of PPM and uncommented the workaround code.
</commit_message>
<xml_diff>
--- a/uft-one-ppm-executive-build-test/Default.xlsx
+++ b/uft-one-ppm-executive-build-test/Default.xlsx
@@ -187,9 +187,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -200,7 +198,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -542,19 +542,19 @@
       </c>
     </row>
     <row>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
-        <v>5</v>
+      <c s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>3</v>
       </c>
-      <c s="2" t="s">
-        <v>2</v>
+      <c s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>